<commit_message>
Décision de codage en python
Import tkinter et 1ere modif de tab
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8505" windowWidth="18195" xWindow="480" yWindow="60"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="162913" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -27,6 +27,7 @@
     </font>
     <font>
       <name val="Inherit"/>
+      <family val="2"/>
       <color rgb="FF676767"/>
       <sz val="11"/>
     </font>
@@ -40,14 +41,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFfcfcfc"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFCFCFC"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFffffff"/>
       </patternFill>
     </fill>
   </fills>
@@ -61,85 +60,99 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </left>
       <right style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color rgb="FFececec"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
       <right style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color rgb="FFececec"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </left>
       <right style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </right>
-      <top style="medium">
-        <color rgb="FFECECEC"/>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
       <right style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </right>
-      <top style="medium">
-        <color rgb="FFECECEC"/>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
       </top>
       <bottom style="medium">
-        <color rgb="FFECECEC"/>
+        <color rgb="FFececec"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+  <cellXfs count="9">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="2" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="4" fillId="3" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="2" fontId="1" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -216,10 +229,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -246,82 +259,82 @@
         <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -333,348 +346,377 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="9500"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot rev="0" lon="0" lat="0"/>
+            </a:camera>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:tint val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="8" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="8" width="14.14785714285714"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>x</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>f(x)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="2" s="1">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="3" s="1">
+      <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="4" s="1">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="5" s="1">
+      <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="7" t="n">
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="6" s="1">
+      <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A7" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="7" s="1">
+      <c r="A7" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="7" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="8" s="1">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="9" s="1">
+      <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="7" t="n">
         <v>49</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="15.75" r="10" s="1">
+      <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>64</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" paperSize="9"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="8" width="14.14785714285714"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="8" width="14.14785714285714"/>
+  </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="inlineStr">
+    <row customFormat="1" customHeight="1" ht="21.75" r="1" s="1">
+      <c r="A1" s="2" t="inlineStr">
         <is>
-          <t>Full Name</t>
+          <t>ca change</t>
         </is>
       </c>
-      <c r="B1" s="6" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>f(x)</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A2" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="2" s="1">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="5" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A3" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="3" s="1">
+      <c r="A3" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="7" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="4" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A4" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="4" s="1">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="n">
+      <c r="B4" s="5" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A5" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="5" s="1">
+      <c r="A5" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="7" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A6" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="6" s="1">
+      <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B6" s="4" t="n">
+      <c r="B6" s="5" t="n">
         <v>64</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A7" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="7" s="1">
+      <c r="A7" s="6" t="n">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="7" t="n">
         <v>125</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A8" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="8" s="1">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B8" s="4" t="n">
+      <c r="B8" s="5" t="n">
         <v>216</v>
       </c>
     </row>
-    <row r="9" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A9" s="1" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="9" s="1">
+      <c r="A9" s="6" t="n">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="7" t="n">
         <v>343</v>
       </c>
     </row>
-    <row r="10" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="3" t="n">
+    <row customFormat="1" customHeight="1" ht="21.75" r="10" s="1">
+      <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B10" s="4" t="n">
+      <c r="B10" s="5" t="n">
         <v>512</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>